<commit_message>
atualiza saude solagos dashboard
</commit_message>
<xml_diff>
--- a/dashboard.xlsx
+++ b/dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\GamErick\Desktop\Nova pasta\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B23EF293-9FD7-42E4-A9A4-94AFD203BC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F043A6B-D746-4C06-890A-F9B765E65F11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="75">
   <si>
     <t>JANEIRO</t>
   </si>
@@ -1315,7 +1315,7 @@
   <dimension ref="A1:R12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1629,11 +1629,11 @@
       <c r="C8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>25</v>
+      <c r="D8" s="2">
+        <v>1932</v>
+      </c>
+      <c r="E8" s="2">
+        <v>2024</v>
       </c>
       <c r="F8" s="2">
         <v>9500</v>
@@ -1641,7 +1641,9 @@
       <c r="G8" s="12">
         <v>8128</v>
       </c>
-      <c r="H8" s="26"/>
+      <c r="H8" s="26">
+        <v>3166</v>
+      </c>
       <c r="I8" s="11"/>
       <c r="J8" s="11"/>
       <c r="K8" s="11"/>
@@ -1653,7 +1655,7 @@
       <c r="Q8" s="11"/>
       <c r="R8" s="14">
         <f t="shared" si="0"/>
-        <v>17628</v>
+        <v>20794</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>